<commit_message>
New training stats and stuff
</commit_message>
<xml_diff>
--- a/Fixed Baselines/results.xlsx
+++ b/Fixed Baselines/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>BigFish</t>
   </si>
@@ -55,7 +55,13 @@
     <t>Miner</t>
   </si>
   <si>
+    <t>Ninja</t>
+  </si>
+  <si>
     <t>Plunder</t>
+  </si>
+  <si>
+    <t>Starpilot</t>
   </si>
   <si>
     <t>steps</t>
@@ -422,13 +428,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,10 +477,16 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>7946240</v>
@@ -507,7 +519,7 @@
         <v>7946240</v>
       </c>
       <c r="L2">
-        <v>5775360</v>
+        <v>7946240</v>
       </c>
       <c r="M2">
         <v>7946240</v>
@@ -518,10 +530,16 @@
       <c r="O2">
         <v>7946240</v>
       </c>
+      <c r="P2">
+        <v>7946240</v>
+      </c>
+      <c r="Q2">
+        <v>7946240</v>
+      </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>5.463541507720947</v>
@@ -554,7 +572,7 @@
         <v>69.89583587646484</v>
       </c>
       <c r="L3">
-        <v>19.921875</v>
+        <v>17.41319465637207</v>
       </c>
       <c r="M3">
         <v>21.21527862548828</v>
@@ -563,12 +581,18 @@
         <v>122.7638854980469</v>
       </c>
       <c r="O3">
+        <v>40.69444274902344</v>
+      </c>
+      <c r="P3">
         <v>4.684027671813965</v>
       </c>
+      <c r="Q3">
+        <v>26.93923568725586</v>
+      </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>2.65625</v>
@@ -601,7 +625,7 @@
         <v>13.97569465637207</v>
       </c>
       <c r="L4">
-        <v>14.921875</v>
+        <v>14.91319465637207</v>
       </c>
       <c r="M4">
         <v>5.24305534362793</v>
@@ -610,7 +634,13 @@
         <v>7.265625</v>
       </c>
       <c r="O4">
+        <v>40.29513931274414</v>
+      </c>
+      <c r="P4">
         <v>4.173611164093018</v>
+      </c>
+      <c r="Q4">
+        <v>26.62847137451172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>